<commit_message>
uhm added a lil thing :3
</commit_message>
<xml_diff>
--- a/triggersheet.xlsx
+++ b/triggersheet.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>&gt;ping</t>
   </si>
@@ -19,29 +19,136 @@
     <t>systems functional, or as it would appear...</t>
   </si>
   <si>
-    <t>&gt;drg</t>
+    <t>drg</t>
   </si>
   <si>
     <t>Deep rock galactic? in MY rat game server?</t>
   </si>
   <si>
-    <t>&gt;dang</t>
+    <t>dang</t>
   </si>
   <si>
     <t>dang, that's crazy</t>
   </si>
   <si>
-    <t>&gt;build</t>
-  </si>
-  <si>
-    <t>[WIP] -&gt; will parse info later</t>
+    <t>hehe</t>
+  </si>
+  <si>
+    <t>:hehe:</t>
+  </si>
+  <si>
+    <t>botting</t>
+  </si>
+  <si>
+    <t>dunno, you tell me</t>
+  </si>
+  <si>
+    <t>crazy</t>
+  </si>
+  <si>
+    <t>Crazy? I was crazy once. They put me in a room. A rubber room. A rubber room with rats. And rats make me crazy.</t>
+  </si>
+  <si>
+    <t>beef</t>
+  </si>
+  <si>
+    <t>what a fabulous slab of beef i am</t>
+  </si>
+  <si>
+    <t>StickyFuel</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="&quot;Roboto Mono&quot;, Arial"/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t xml:space="preserve">Sticky Fuel is one of the best and most reliable wave clear tools in the game. With great attention economy, it takes care of swarmers and grunts and provides, if built like this, slow on everything else. To play it, lay flames on the floor/walls trying to predict bugs' paths or while kiting. 
+A note on T5: T5B is generally preferred to T5A with Sticky Fuel since it's hard to use heat radiance with the low magazine size of this build, plus it helps with jellies and shredders in tight spaces. Sticky Fuel discussion: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="&quot;Roboto Mono&quot;, Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t>Link</t>
+    </r>
+  </si>
+  <si>
+    <t>FuelStreamDiffuser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hybrid build that plays similar to Sticky Fuel but makes use of heat radiance. It's easier to play than Sticky for beginners due to the more direct playstyle and increased range. One of its more niche uses is to heat patrol bots and sentries in Sabotage or Rival Incursion missions. </t>
+  </si>
+  <si>
+    <t>DisperserCompound</t>
+  </si>
+  <si>
+    <t>Slightly weaker alternative to Sticky Fuel in DPS but provides a better slow. Floor coverage can be better than Sticky but Sludge has trouble covering walls and ceilings. One of its advantages is being able to cover areas that are far away by aiming a charged shot, which is useful in certain situations like the Hearthstone fight or in general when fighting in open terrain.</t>
+  </si>
+  <si>
+    <t>VolatileImpactMixture</t>
+  </si>
+  <si>
+    <t>Slightly weaker alternative to Sticky Fuel, more focused on single-target damage.</t>
+  </si>
+  <si>
+    <t>SludgeBlast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single-target damage focused build, good for some variety in elimination / sabotage. Ammo economy is poor and the teammates will have to cover the loss of Driller's wave clear depending on the difficulty. </t>
+  </si>
+  <si>
+    <t>ImprovedThermalEfficiency</t>
+  </si>
+  <si>
+    <t>The staple of cryo comps, it is also a common pick in Elimination missions to freeze the dreadnoughts. Take ITE for general use and Snowball for an easier time dealing with macteras and chunks of high-HP grouped enemies such as sentinels.</t>
+  </si>
+  <si>
+    <t>FSD</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>VIM</t>
+  </si>
+  <si>
+    <t>ITE</t>
+  </si>
+  <si>
+    <t>Sticky</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="&quot;Roboto Mono&quot;, Arial"/>
+        <color theme="1"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t xml:space="preserve">Sticky Fuel is one of the best and most reliable wave clear tools in the game. With great attention economy, it takes care of swarmers and grunts and provides, if built like this, slow on everything else. To play it, lay flames on the floor/walls trying to predict bugs' paths or while kiting. 
+A note on T5: T5B is generally preferred to T5A with Sticky Fuel since it's hard to use heat radiance with the low magazine size of this build, plus it helps with jellies and shredders in tight spaces. Sticky Fuel discussion: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="&quot;Roboto Mono&quot;, Arial"/>
+        <color rgb="FF000000"/>
+        <sz val="9.0"/>
+      </rPr>
+      <t>Link</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -53,28 +160,168 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="&quot;Roboto Mono&quot;"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color theme="1"/>
+      <name val="&quot;Roboto Mono&quot;"/>
+    </font>
+    <font/>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF3F3F3"/>
+        <bgColor rgb="FFF3F3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FFB7B7B7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB7B7B7"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB7B7B7"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB7B7B7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FFB7B7B7"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FFB7B7B7"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB7B7B7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB7B7B7"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FFB7B7B7"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -292,6 +539,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="2" max="2" width="113.5"/>
+    <col customWidth="1" min="3" max="3" width="56.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -326,7 +574,149 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" ht="48.75" customHeight="1">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="12"/>
+      <c r="B15" s="13"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+  </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>